<commit_message>
updated the columns headers as an option, added fillnas option for no extra pivoted columns (veh_no) and added a summary statistic function to be applied per main category in columns
</commit_message>
<xml_diff>
--- a/kc/kc_data_dict.xlsx
+++ b/kc/kc_data_dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Documents\Classes\W210 - Capstone\NYCTrafficCollisions\kc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324C849B-9F9B-4332-BA05-3A7F3122F7AC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E45D8C-5608-408D-AFBD-5FFD42A6C33B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8025" xr2:uid="{895D2BAD-501D-4616-9672-884AC9F0551D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11880" xr2:uid="{895D2BAD-501D-4616-9672-884AC9F0551D}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="287">
   <si>
     <t>Variable</t>
   </si>
@@ -209,9 +209,6 @@
     <t>Vehicle Traveling Speed</t>
   </si>
   <si>
-    <t>&gt;151mph</t>
-  </si>
-  <si>
     <t>underride</t>
   </si>
   <si>
@@ -800,9 +797,6 @@
     <t>6, 10, 11, 12, 15</t>
   </si>
   <si>
-    <t>9999 = all else</t>
-  </si>
-  <si>
     <t>998,999</t>
   </si>
   <si>
@@ -891,14 +885,25 @@
   </si>
   <si>
     <t>Numeric</t>
+  </si>
+  <si>
+    <t>9999 = all else (this should always be the LAST category)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -926,13 +931,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1249,8 +1255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66FB29DA-B7F0-47F0-877E-10B77E041BFB}">
   <dimension ref="A1:I217"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1259,7 +1265,8 @@
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="6" max="7" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1273,7 +1280,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -1287,8 +1294,8 @@
       <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
-        <v>257</v>
+      <c r="I1" s="6" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1304,11 +1311,11 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
-        <v>285</v>
-      </c>
       <c r="H2" t="s">
-        <v>235</v>
+        <v>283</v>
+      </c>
+      <c r="I2" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1327,11 +1334,11 @@
       <c r="E3">
         <v>99</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3">
+        <v>99</v>
+      </c>
+      <c r="H3" t="s">
         <v>9</v>
-      </c>
-      <c r="G3">
-        <v>9999</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1420,10 +1427,10 @@
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1446,7 +1453,7 @@
         <v>25</v>
       </c>
       <c r="G8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1579,7 +1586,7 @@
       </c>
       <c r="E14" s="1"/>
       <c r="H14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1625,7 +1632,7 @@
         <v>35</v>
       </c>
       <c r="G16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1648,7 +1655,7 @@
         <v>36</v>
       </c>
       <c r="G17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1717,7 +1724,7 @@
         <v>44</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1740,7 +1747,7 @@
         <v>46</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1763,7 +1770,7 @@
         <v>37</v>
       </c>
       <c r="G22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1786,7 +1793,7 @@
         <v>45</v>
       </c>
       <c r="G23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1826,13 +1833,13 @@
         <v>15</v>
       </c>
       <c r="E25">
-        <v>11</v>
+        <v>99</v>
       </c>
       <c r="F25" t="s">
-        <v>48</v>
-      </c>
-      <c r="G25">
-        <v>9999</v>
+        <v>47</v>
+      </c>
+      <c r="G25" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1849,13 +1856,13 @@
         <v>15</v>
       </c>
       <c r="E26">
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="F26" t="s">
-        <v>47</v>
-      </c>
-      <c r="G26" t="s">
-        <v>96</v>
+        <v>48</v>
+      </c>
+      <c r="G26">
+        <v>9999</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1863,13 +1870,13 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C27" t="s">
         <v>49</v>
       </c>
       <c r="D27" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1952,7 +1959,7 @@
         <v>59</v>
       </c>
       <c r="D31" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1971,14 +1978,14 @@
       <c r="E32">
         <v>152</v>
       </c>
-      <c r="F32" t="s">
-        <v>60</v>
+      <c r="F32">
+        <v>152</v>
       </c>
       <c r="G32">
         <v>997</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -1994,22 +2001,22 @@
       <c r="E33">
         <v>999</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="H33" t="s">
         <v>47</v>
       </c>
-      <c r="G33" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>6</v>
       </c>
       <c r="B34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" t="s">
         <v>63</v>
-      </c>
-      <c r="C34" t="s">
-        <v>64</v>
       </c>
       <c r="D34" t="s">
         <v>15</v>
@@ -2024,15 +2031,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>6</v>
       </c>
       <c r="B35" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" t="s">
         <v>63</v>
-      </c>
-      <c r="C35" t="s">
-        <v>64</v>
       </c>
       <c r="D35" t="s">
         <v>15</v>
@@ -2044,18 +2051,18 @@
         <v>17</v>
       </c>
       <c r="G35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>66</v>
-      </c>
-      <c r="C36" t="s">
-        <v>67</v>
       </c>
       <c r="D36" t="s">
         <v>15</v>
@@ -2070,15 +2077,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>6</v>
       </c>
       <c r="B37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" t="s">
         <v>66</v>
-      </c>
-      <c r="C37" t="s">
-        <v>67</v>
       </c>
       <c r="D37" t="s">
         <v>15</v>
@@ -2087,90 +2094,90 @@
         <v>1</v>
       </c>
       <c r="F37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G37" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>6</v>
       </c>
       <c r="B38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" t="s">
         <v>66</v>
       </c>
-      <c r="C38" t="s">
-        <v>67</v>
-      </c>
       <c r="D38" t="s">
         <v>15</v>
       </c>
       <c r="E38">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F38" t="s">
         <v>69</v>
       </c>
       <c r="G38">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39" t="s">
+        <v>68</v>
+      </c>
+      <c r="G39">
         <v>9999</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>6</v>
-      </c>
-      <c r="B39" t="s">
-        <v>66</v>
-      </c>
-      <c r="C39" t="s">
-        <v>67</v>
-      </c>
-      <c r="D39" t="s">
-        <v>15</v>
-      </c>
-      <c r="E39">
-        <v>9</v>
-      </c>
-      <c r="F39" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" t="s">
         <v>70</v>
       </c>
-      <c r="G39">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>6</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>71</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40">
+        <v>6</v>
+      </c>
+      <c r="F40" t="s">
         <v>72</v>
       </c>
-      <c r="D40" t="s">
-        <v>15</v>
-      </c>
-      <c r="E40">
-        <v>6</v>
-      </c>
-      <c r="F40" t="s">
-        <v>73</v>
-      </c>
       <c r="G40">
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>6</v>
       </c>
       <c r="B41" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" t="s">
         <v>71</v>
-      </c>
-      <c r="C41" t="s">
-        <v>72</v>
       </c>
       <c r="D41" t="s">
         <v>15</v>
@@ -2179,21 +2186,21 @@
         <v>4</v>
       </c>
       <c r="F41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G41">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>6</v>
       </c>
       <c r="B42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" t="s">
         <v>71</v>
-      </c>
-      <c r="C42" t="s">
-        <v>72</v>
       </c>
       <c r="D42" t="s">
         <v>15</v>
@@ -2202,21 +2209,21 @@
         <v>2</v>
       </c>
       <c r="F42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G42">
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>6</v>
       </c>
       <c r="B43" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" t="s">
         <v>71</v>
-      </c>
-      <c r="C43" t="s">
-        <v>72</v>
       </c>
       <c r="D43" t="s">
         <v>15</v>
@@ -2225,21 +2232,21 @@
         <v>9</v>
       </c>
       <c r="F43" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G43">
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>6</v>
       </c>
       <c r="B44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" t="s">
         <v>71</v>
-      </c>
-      <c r="C44" t="s">
-        <v>72</v>
       </c>
       <c r="D44" t="s">
         <v>15</v>
@@ -2248,21 +2255,21 @@
         <v>0</v>
       </c>
       <c r="F44" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G44">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>6</v>
       </c>
       <c r="B45" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" t="s">
         <v>77</v>
-      </c>
-      <c r="C45" t="s">
-        <v>78</v>
       </c>
       <c r="D45" t="s">
         <v>15</v>
@@ -2271,21 +2278,21 @@
         <v>12</v>
       </c>
       <c r="F45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G45">
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>6</v>
       </c>
       <c r="B46" t="s">
+        <v>76</v>
+      </c>
+      <c r="C46" t="s">
         <v>77</v>
-      </c>
-      <c r="C46" t="s">
-        <v>78</v>
       </c>
       <c r="D46" t="s">
         <v>15</v>
@@ -2294,21 +2301,21 @@
         <v>8</v>
       </c>
       <c r="F46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G46">
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>6</v>
       </c>
       <c r="B47" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47" t="s">
         <v>77</v>
-      </c>
-      <c r="C47" t="s">
-        <v>78</v>
       </c>
       <c r="D47" t="s">
         <v>15</v>
@@ -2317,21 +2324,21 @@
         <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G47">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>6</v>
       </c>
       <c r="B48" t="s">
+        <v>76</v>
+      </c>
+      <c r="C48" t="s">
         <v>77</v>
-      </c>
-      <c r="C48" t="s">
-        <v>78</v>
       </c>
       <c r="D48" t="s">
         <v>15</v>
@@ -2340,7 +2347,7 @@
         <v>42</v>
       </c>
       <c r="F48" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G48">
         <v>42</v>
@@ -2351,22 +2358,22 @@
         <v>6</v>
       </c>
       <c r="B49" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49" t="s">
         <v>77</v>
       </c>
-      <c r="C49" t="s">
-        <v>78</v>
-      </c>
       <c r="D49" t="s">
         <v>15</v>
       </c>
       <c r="E49">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F49" t="s">
-        <v>48</v>
+        <v>83</v>
       </c>
       <c r="G49">
-        <v>9999</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -2374,22 +2381,22 @@
         <v>6</v>
       </c>
       <c r="B50" t="s">
+        <v>76</v>
+      </c>
+      <c r="C50" t="s">
         <v>77</v>
       </c>
-      <c r="C50" t="s">
-        <v>78</v>
-      </c>
       <c r="D50" t="s">
         <v>15</v>
       </c>
       <c r="E50">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F50" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="G50">
-        <v>99</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -2397,10 +2404,10 @@
         <v>6</v>
       </c>
       <c r="B51" t="s">
+        <v>84</v>
+      </c>
+      <c r="C51" t="s">
         <v>85</v>
-      </c>
-      <c r="C51" t="s">
-        <v>86</v>
       </c>
       <c r="D51" t="s">
         <v>15</v>
@@ -2409,7 +2416,7 @@
         <v>0</v>
       </c>
       <c r="F51" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G51">
         <v>0</v>
@@ -2420,10 +2427,10 @@
         <v>6</v>
       </c>
       <c r="B52" t="s">
+        <v>84</v>
+      </c>
+      <c r="C52" t="s">
         <v>85</v>
-      </c>
-      <c r="C52" t="s">
-        <v>86</v>
       </c>
       <c r="D52" t="s">
         <v>15</v>
@@ -2432,7 +2439,7 @@
         <v>1</v>
       </c>
       <c r="F52" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G52">
         <v>1</v>
@@ -2443,10 +2450,10 @@
         <v>6</v>
       </c>
       <c r="B53" t="s">
+        <v>84</v>
+      </c>
+      <c r="C53" t="s">
         <v>85</v>
-      </c>
-      <c r="C53" t="s">
-        <v>86</v>
       </c>
       <c r="D53" t="s">
         <v>15</v>
@@ -2455,10 +2462,10 @@
         <v>2</v>
       </c>
       <c r="F53" t="s">
+        <v>89</v>
+      </c>
+      <c r="G53" t="s">
         <v>90</v>
-      </c>
-      <c r="G53" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -2466,10 +2473,10 @@
         <v>6</v>
       </c>
       <c r="B54" t="s">
+        <v>84</v>
+      </c>
+      <c r="C54" t="s">
         <v>85</v>
-      </c>
-      <c r="C54" t="s">
-        <v>86</v>
       </c>
       <c r="D54" t="s">
         <v>15</v>
@@ -2478,7 +2485,7 @@
         <v>3</v>
       </c>
       <c r="F54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G54">
         <v>3</v>
@@ -2489,10 +2496,10 @@
         <v>6</v>
       </c>
       <c r="B55" t="s">
+        <v>84</v>
+      </c>
+      <c r="C55" t="s">
         <v>85</v>
-      </c>
-      <c r="C55" t="s">
-        <v>86</v>
       </c>
       <c r="D55" t="s">
         <v>15</v>
@@ -2501,7 +2508,7 @@
         <v>4</v>
       </c>
       <c r="F55" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G55">
         <v>4</v>
@@ -2512,11 +2519,11 @@
         <v>6</v>
       </c>
       <c r="B56" t="s">
+        <v>84</v>
+      </c>
+      <c r="C56" t="s">
         <v>85</v>
       </c>
-      <c r="C56" t="s">
-        <v>86</v>
-      </c>
       <c r="D56" t="s">
         <v>15</v>
       </c>
@@ -2524,7 +2531,7 @@
         <v>6</v>
       </c>
       <c r="F56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G56">
         <v>6</v>
@@ -2535,10 +2542,10 @@
         <v>6</v>
       </c>
       <c r="B57" t="s">
+        <v>84</v>
+      </c>
+      <c r="C57" t="s">
         <v>85</v>
-      </c>
-      <c r="C57" t="s">
-        <v>86</v>
       </c>
       <c r="D57" t="s">
         <v>15</v>
@@ -2550,7 +2557,7 @@
         <v>47</v>
       </c>
       <c r="G57" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -2558,16 +2565,16 @@
         <v>6</v>
       </c>
       <c r="B58" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C58" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D58" t="s">
         <v>10</v>
       </c>
       <c r="H58" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -2575,10 +2582,10 @@
         <v>6</v>
       </c>
       <c r="B59" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C59" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D59" t="s">
         <v>10</v>
@@ -2586,11 +2593,11 @@
       <c r="E59">
         <v>99</v>
       </c>
-      <c r="F59" t="s">
+      <c r="G59" t="s">
+        <v>93</v>
+      </c>
+      <c r="H59" t="s">
         <v>47</v>
-      </c>
-      <c r="G59" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -2598,16 +2605,16 @@
         <v>6</v>
       </c>
       <c r="B60" t="s">
+        <v>97</v>
+      </c>
+      <c r="C60" t="s">
         <v>98</v>
-      </c>
-      <c r="C60" t="s">
-        <v>99</v>
       </c>
       <c r="D60" t="s">
         <v>10</v>
       </c>
       <c r="H60" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -2615,10 +2622,10 @@
         <v>6</v>
       </c>
       <c r="B61" t="s">
+        <v>97</v>
+      </c>
+      <c r="C61" t="s">
         <v>98</v>
-      </c>
-      <c r="C61" t="s">
-        <v>99</v>
       </c>
       <c r="D61" t="s">
         <v>10</v>
@@ -2626,11 +2633,11 @@
       <c r="E61">
         <v>99</v>
       </c>
-      <c r="F61" t="s">
+      <c r="G61" t="s">
+        <v>95</v>
+      </c>
+      <c r="H61" t="s">
         <v>47</v>
-      </c>
-      <c r="G61" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -2638,10 +2645,10 @@
         <v>6</v>
       </c>
       <c r="B62" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C62" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D62" t="s">
         <v>15</v>
@@ -2650,7 +2657,7 @@
         <v>0</v>
       </c>
       <c r="F62" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G62">
         <v>0</v>
@@ -2661,10 +2668,10 @@
         <v>6</v>
       </c>
       <c r="B63" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C63" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D63" t="s">
         <v>15</v>
@@ -2673,7 +2680,7 @@
         <v>1</v>
       </c>
       <c r="F63" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G63">
         <v>1</v>
@@ -2684,10 +2691,10 @@
         <v>6</v>
       </c>
       <c r="B64" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C64" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D64" t="s">
         <v>15</v>
@@ -2696,10 +2703,10 @@
         <v>2</v>
       </c>
       <c r="F64" t="s">
+        <v>104</v>
+      </c>
+      <c r="G64" t="s">
         <v>105</v>
-      </c>
-      <c r="G64" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -2707,10 +2714,10 @@
         <v>6</v>
       </c>
       <c r="B65" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C65" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D65" t="s">
         <v>15</v>
@@ -2722,7 +2729,7 @@
         <v>47</v>
       </c>
       <c r="G65" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -2730,10 +2737,10 @@
         <v>6</v>
       </c>
       <c r="B66" t="s">
+        <v>106</v>
+      </c>
+      <c r="C66" t="s">
         <v>107</v>
-      </c>
-      <c r="C66" t="s">
-        <v>108</v>
       </c>
       <c r="D66" t="s">
         <v>15</v>
@@ -2742,7 +2749,7 @@
         <v>0</v>
       </c>
       <c r="F66" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G66">
         <v>0</v>
@@ -2753,10 +2760,10 @@
         <v>6</v>
       </c>
       <c r="B67" t="s">
+        <v>106</v>
+      </c>
+      <c r="C67" t="s">
         <v>107</v>
-      </c>
-      <c r="C67" t="s">
-        <v>108</v>
       </c>
       <c r="D67" t="s">
         <v>15</v>
@@ -2765,7 +2772,7 @@
         <v>1</v>
       </c>
       <c r="F67" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G67">
         <v>1</v>
@@ -2776,22 +2783,22 @@
         <v>6</v>
       </c>
       <c r="B68" t="s">
+        <v>106</v>
+      </c>
+      <c r="C68" t="s">
         <v>107</v>
       </c>
-      <c r="C68" t="s">
-        <v>108</v>
-      </c>
       <c r="D68" t="s">
         <v>15</v>
       </c>
       <c r="E68">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F68" t="s">
-        <v>110</v>
-      </c>
-      <c r="G68">
-        <v>9999</v>
+        <v>47</v>
+      </c>
+      <c r="G68" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -2799,22 +2806,22 @@
         <v>6</v>
       </c>
       <c r="B69" t="s">
+        <v>106</v>
+      </c>
+      <c r="C69" t="s">
         <v>107</v>
       </c>
-      <c r="C69" t="s">
-        <v>108</v>
-      </c>
       <c r="D69" t="s">
         <v>15</v>
       </c>
       <c r="E69">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F69" t="s">
-        <v>47</v>
-      </c>
-      <c r="G69" t="s">
-        <v>94</v>
+        <v>109</v>
+      </c>
+      <c r="G69">
+        <v>9999</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -2822,10 +2829,10 @@
         <v>6</v>
       </c>
       <c r="B70" t="s">
+        <v>112</v>
+      </c>
+      <c r="C70" t="s">
         <v>113</v>
-      </c>
-      <c r="C70" t="s">
-        <v>114</v>
       </c>
       <c r="D70" t="s">
         <v>15</v>
@@ -2834,7 +2841,7 @@
         <v>0</v>
       </c>
       <c r="F70" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -2845,10 +2852,10 @@
         <v>6</v>
       </c>
       <c r="B71" t="s">
+        <v>112</v>
+      </c>
+      <c r="C71" t="s">
         <v>113</v>
-      </c>
-      <c r="C71" t="s">
-        <v>114</v>
       </c>
       <c r="D71" t="s">
         <v>15</v>
@@ -2857,7 +2864,7 @@
         <v>1</v>
       </c>
       <c r="F71" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G71">
         <v>1</v>
@@ -2868,10 +2875,10 @@
         <v>6</v>
       </c>
       <c r="B72" t="s">
+        <v>112</v>
+      </c>
+      <c r="C72" t="s">
         <v>113</v>
-      </c>
-      <c r="C72" t="s">
-        <v>114</v>
       </c>
       <c r="D72" t="s">
         <v>15</v>
@@ -2880,10 +2887,10 @@
         <v>2</v>
       </c>
       <c r="F72" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G72" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2891,10 +2898,10 @@
         <v>6</v>
       </c>
       <c r="B73" t="s">
+        <v>112</v>
+      </c>
+      <c r="C73" t="s">
         <v>113</v>
-      </c>
-      <c r="C73" t="s">
-        <v>114</v>
       </c>
       <c r="D73" t="s">
         <v>15</v>
@@ -2903,10 +2910,10 @@
         <v>3</v>
       </c>
       <c r="F73" t="s">
+        <v>115</v>
+      </c>
+      <c r="G73" t="s">
         <v>116</v>
-      </c>
-      <c r="G73" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -2914,10 +2921,10 @@
         <v>6</v>
       </c>
       <c r="B74" t="s">
+        <v>112</v>
+      </c>
+      <c r="C74" t="s">
         <v>113</v>
-      </c>
-      <c r="C74" t="s">
-        <v>114</v>
       </c>
       <c r="D74" t="s">
         <v>15</v>
@@ -2926,10 +2933,10 @@
         <v>4</v>
       </c>
       <c r="F74" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G74" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -2937,10 +2944,10 @@
         <v>6</v>
       </c>
       <c r="B75" t="s">
+        <v>112</v>
+      </c>
+      <c r="C75" t="s">
         <v>113</v>
-      </c>
-      <c r="C75" t="s">
-        <v>114</v>
       </c>
       <c r="D75" t="s">
         <v>15</v>
@@ -2949,10 +2956,10 @@
         <v>5</v>
       </c>
       <c r="F75" t="s">
+        <v>120</v>
+      </c>
+      <c r="G75" t="s">
         <v>121</v>
-      </c>
-      <c r="G75" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2960,10 +2967,10 @@
         <v>6</v>
       </c>
       <c r="B76" t="s">
+        <v>112</v>
+      </c>
+      <c r="C76" t="s">
         <v>113</v>
-      </c>
-      <c r="C76" t="s">
-        <v>114</v>
       </c>
       <c r="D76" t="s">
         <v>15</v>
@@ -2975,7 +2982,7 @@
         <v>47</v>
       </c>
       <c r="G76" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2983,10 +2990,10 @@
         <v>6</v>
       </c>
       <c r="B77" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C77" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D77" t="s">
         <v>15</v>
@@ -2995,7 +3002,7 @@
         <v>0</v>
       </c>
       <c r="F77" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G77">
         <v>0</v>
@@ -3006,10 +3013,10 @@
         <v>6</v>
       </c>
       <c r="B78" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C78" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D78" t="s">
         <v>15</v>
@@ -3018,10 +3025,10 @@
         <v>1</v>
       </c>
       <c r="F78" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -3029,10 +3036,10 @@
         <v>6</v>
       </c>
       <c r="B79" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C79" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D79" t="s">
         <v>15</v>
@@ -3041,7 +3048,7 @@
         <v>20</v>
       </c>
       <c r="F79" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G79">
         <v>20</v>
@@ -3052,10 +3059,10 @@
         <v>6</v>
       </c>
       <c r="B80" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C80" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D80" t="s">
         <v>15</v>
@@ -3064,10 +3071,10 @@
         <v>21</v>
       </c>
       <c r="F80" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -3075,10 +3082,10 @@
         <v>6</v>
       </c>
       <c r="B81" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C81" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D81" t="s">
         <v>15</v>
@@ -3087,7 +3094,7 @@
         <v>40</v>
       </c>
       <c r="F81" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G81">
         <v>40</v>
@@ -3098,22 +3105,22 @@
         <v>6</v>
       </c>
       <c r="B82" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C82" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D82" t="s">
         <v>15</v>
       </c>
       <c r="E82">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="F82" t="s">
+        <v>47</v>
+      </c>
+      <c r="G82" t="s">
         <v>131</v>
-      </c>
-      <c r="G82">
-        <v>9999</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -3121,22 +3128,22 @@
         <v>6</v>
       </c>
       <c r="B83" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C83" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D83" t="s">
         <v>15</v>
       </c>
       <c r="E83">
-        <v>99</v>
+        <v>41</v>
       </c>
       <c r="F83" t="s">
-        <v>47</v>
-      </c>
-      <c r="G83" t="s">
-        <v>132</v>
+        <v>130</v>
+      </c>
+      <c r="G83">
+        <v>9999</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -3144,10 +3151,10 @@
         <v>6</v>
       </c>
       <c r="B84" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C84" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D84" t="s">
         <v>15</v>
@@ -3156,7 +3163,7 @@
         <v>0</v>
       </c>
       <c r="F84" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G84">
         <v>0</v>
@@ -3167,10 +3174,10 @@
         <v>6</v>
       </c>
       <c r="B85" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C85" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D85" t="s">
         <v>15</v>
@@ -3179,7 +3186,7 @@
         <v>3</v>
       </c>
       <c r="F85" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G85">
         <v>3</v>
@@ -3190,10 +3197,10 @@
         <v>6</v>
       </c>
       <c r="B86" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C86" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D86" t="s">
         <v>15</v>
@@ -3202,10 +3209,10 @@
         <v>1</v>
       </c>
       <c r="F86" t="s">
+        <v>135</v>
+      </c>
+      <c r="G86" t="s">
         <v>136</v>
-      </c>
-      <c r="G86" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -3213,10 +3220,10 @@
         <v>6</v>
       </c>
       <c r="B87" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C87" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D87" t="s">
         <v>15</v>
@@ -3228,7 +3235,7 @@
         <v>47</v>
       </c>
       <c r="G87" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -3236,10 +3243,10 @@
         <v>6</v>
       </c>
       <c r="B88" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C88" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D88" t="s">
         <v>15</v>
@@ -3248,7 +3255,7 @@
         <v>0</v>
       </c>
       <c r="F88" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G88">
         <v>0</v>
@@ -3259,10 +3266,10 @@
         <v>6</v>
       </c>
       <c r="B89" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C89" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D89" t="s">
         <v>15</v>
@@ -3271,7 +3278,7 @@
         <v>1</v>
       </c>
       <c r="F89" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G89">
         <v>1</v>
@@ -3282,10 +3289,10 @@
         <v>6</v>
       </c>
       <c r="B90" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C90" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D90" t="s">
         <v>15</v>
@@ -3294,10 +3301,10 @@
         <v>2</v>
       </c>
       <c r="F90" t="s">
+        <v>142</v>
+      </c>
+      <c r="G90" t="s">
         <v>143</v>
-      </c>
-      <c r="G90" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -3305,10 +3312,10 @@
         <v>6</v>
       </c>
       <c r="B91" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C91" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D91" t="s">
         <v>15</v>
@@ -3317,7 +3324,7 @@
         <v>7</v>
       </c>
       <c r="F91" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G91">
         <v>7</v>
@@ -3328,10 +3335,10 @@
         <v>6</v>
       </c>
       <c r="B92" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C92" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D92" t="s">
         <v>15</v>
@@ -3340,7 +3347,7 @@
         <v>9</v>
       </c>
       <c r="F92" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G92">
         <v>9</v>
@@ -3351,10 +3358,10 @@
         <v>6</v>
       </c>
       <c r="B93" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C93" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D93" t="s">
         <v>15</v>
@@ -3363,7 +3370,7 @@
         <v>0</v>
       </c>
       <c r="F93" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G93">
         <v>0</v>
@@ -3374,10 +3381,10 @@
         <v>6</v>
       </c>
       <c r="B94" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C94" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D94" t="s">
         <v>15</v>
@@ -3386,10 +3393,10 @@
         <v>1</v>
       </c>
       <c r="F94" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G94" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -3397,10 +3404,10 @@
         <v>6</v>
       </c>
       <c r="B95" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C95" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D95" t="s">
         <v>15</v>
@@ -3409,7 +3416,7 @@
         <v>5</v>
       </c>
       <c r="F95" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G95">
         <v>5</v>
@@ -3420,10 +3427,10 @@
         <v>6</v>
       </c>
       <c r="B96" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C96" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D96" t="s">
         <v>15</v>
@@ -3432,7 +3439,7 @@
         <v>6</v>
       </c>
       <c r="F96" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G96">
         <v>6</v>
@@ -3443,10 +3450,10 @@
         <v>6</v>
       </c>
       <c r="B97" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C97" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D97" t="s">
         <v>15</v>
@@ -3455,7 +3462,7 @@
         <v>10</v>
       </c>
       <c r="F97" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G97">
         <v>10</v>
@@ -3466,10 +3473,10 @@
         <v>6</v>
       </c>
       <c r="B98" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C98" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D98" t="s">
         <v>15</v>
@@ -3478,7 +3485,7 @@
         <v>11</v>
       </c>
       <c r="F98" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G98">
         <v>11</v>
@@ -3489,10 +3496,10 @@
         <v>6</v>
       </c>
       <c r="B99" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C99" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D99" t="s">
         <v>15</v>
@@ -3501,7 +3508,7 @@
         <v>15</v>
       </c>
       <c r="F99" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G99">
         <v>15</v>
@@ -3512,10 +3519,10 @@
         <v>6</v>
       </c>
       <c r="B100" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C100" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D100" t="s">
         <v>15</v>
@@ -3524,7 +3531,7 @@
         <v>2</v>
       </c>
       <c r="F100" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G100">
         <v>2</v>
@@ -3535,10 +3542,10 @@
         <v>6</v>
       </c>
       <c r="B101" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C101" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D101" t="s">
         <v>15</v>
@@ -3547,7 +3554,7 @@
         <v>3</v>
       </c>
       <c r="F101" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G101">
         <v>3</v>
@@ -3558,22 +3565,22 @@
         <v>6</v>
       </c>
       <c r="B102" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C102" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D102" t="s">
         <v>15</v>
       </c>
       <c r="E102">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="F102" t="s">
-        <v>48</v>
-      </c>
-      <c r="G102">
-        <v>9999</v>
+        <v>47</v>
+      </c>
+      <c r="G102" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -3581,22 +3588,22 @@
         <v>6</v>
       </c>
       <c r="B103" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C103" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D103" t="s">
         <v>15</v>
       </c>
       <c r="E103">
-        <v>99</v>
+        <v>20</v>
       </c>
       <c r="F103" t="s">
-        <v>47</v>
-      </c>
-      <c r="G103" t="s">
-        <v>96</v>
+        <v>48</v>
+      </c>
+      <c r="G103">
+        <v>9999</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -3604,10 +3611,10 @@
         <v>6</v>
       </c>
       <c r="B104" t="s">
+        <v>157</v>
+      </c>
+      <c r="C104" t="s">
         <v>158</v>
-      </c>
-      <c r="C104" t="s">
-        <v>159</v>
       </c>
       <c r="D104" t="s">
         <v>15</v>
@@ -3616,13 +3623,13 @@
         <v>1</v>
       </c>
       <c r="F104" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G104">
         <v>1</v>
       </c>
       <c r="H104" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -3634,7 +3641,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C105" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D105" t="s">
         <v>15</v>
@@ -3643,13 +3650,13 @@
         <v>2</v>
       </c>
       <c r="F105" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G105">
         <v>2</v>
       </c>
       <c r="H105" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -3661,7 +3668,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C106" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D106" t="s">
         <v>15</v>
@@ -3670,13 +3677,13 @@
         <v>3</v>
       </c>
       <c r="F106" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G106">
         <v>3</v>
       </c>
       <c r="H106" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -3688,7 +3695,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C107" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D107" t="s">
         <v>15</v>
@@ -3697,13 +3704,13 @@
         <v>4</v>
       </c>
       <c r="F107" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G107">
         <v>4</v>
       </c>
       <c r="H107" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -3715,7 +3722,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C108" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D108" t="s">
         <v>15</v>
@@ -3724,13 +3731,13 @@
         <v>5</v>
       </c>
       <c r="F108" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G108">
         <v>5</v>
       </c>
       <c r="H108" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -3742,7 +3749,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C109" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D109" t="s">
         <v>15</v>
@@ -3751,13 +3758,13 @@
         <v>6</v>
       </c>
       <c r="F109" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G109">
         <v>6</v>
       </c>
       <c r="H109" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -3769,7 +3776,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C110" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D110" t="s">
         <v>15</v>
@@ -3778,13 +3785,13 @@
         <v>8</v>
       </c>
       <c r="F110" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G110">
         <v>8</v>
       </c>
       <c r="H110" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -3796,7 +3803,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C111" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D111" t="s">
         <v>15</v>
@@ -3805,13 +3812,13 @@
         <v>9</v>
       </c>
       <c r="F111" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G111">
         <v>9</v>
       </c>
       <c r="H111" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -3823,7 +3830,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C112" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D112" t="s">
         <v>15</v>
@@ -3832,13 +3839,13 @@
         <v>10</v>
       </c>
       <c r="F112" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G112">
         <v>10</v>
       </c>
       <c r="H112" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -3850,7 +3857,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C113" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D113" t="s">
         <v>15</v>
@@ -3859,13 +3866,13 @@
         <v>11</v>
       </c>
       <c r="F113" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G113">
         <v>11</v>
       </c>
       <c r="H113" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -3877,7 +3884,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C114" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D114" t="s">
         <v>15</v>
@@ -3886,13 +3893,13 @@
         <v>12</v>
       </c>
       <c r="F114" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G114">
         <v>12</v>
       </c>
       <c r="H114" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -3904,7 +3911,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C115" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D115" t="s">
         <v>15</v>
@@ -3913,13 +3920,13 @@
         <v>12</v>
       </c>
       <c r="F115" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G115">
         <v>12</v>
       </c>
       <c r="H115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -3931,7 +3938,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C116" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D116" t="s">
         <v>15</v>
@@ -3940,13 +3947,13 @@
         <v>13</v>
       </c>
       <c r="F116" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G116">
         <v>13</v>
       </c>
       <c r="H116" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -3958,7 +3965,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C117" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D117" t="s">
         <v>15</v>
@@ -3967,13 +3974,13 @@
         <v>14</v>
       </c>
       <c r="F117" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G117">
         <v>14</v>
       </c>
       <c r="H117" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -3985,7 +3992,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C118" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D118" t="s">
         <v>15</v>
@@ -3994,13 +4001,13 @@
         <v>15</v>
       </c>
       <c r="F118" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G118">
         <v>15</v>
       </c>
       <c r="H118" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -4012,7 +4019,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C119" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D119" t="s">
         <v>15</v>
@@ -4021,13 +4028,13 @@
         <v>16</v>
       </c>
       <c r="F119" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G119">
         <v>16</v>
       </c>
       <c r="H119" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -4039,7 +4046,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C120" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D120" t="s">
         <v>15</v>
@@ -4048,13 +4055,13 @@
         <v>17</v>
       </c>
       <c r="F120" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G120">
         <v>17</v>
       </c>
       <c r="H120" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -4066,7 +4073,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C121" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D121" t="s">
         <v>15</v>
@@ -4075,13 +4082,13 @@
         <v>18</v>
       </c>
       <c r="F121" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G121">
         <v>18</v>
       </c>
       <c r="H121" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -4093,7 +4100,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C122" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D122" t="s">
         <v>15</v>
@@ -4102,13 +4109,13 @@
         <v>19</v>
       </c>
       <c r="F122" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G122">
         <v>19</v>
       </c>
       <c r="H122" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -4120,7 +4127,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C123" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D123" t="s">
         <v>15</v>
@@ -4129,13 +4136,13 @@
         <v>20</v>
       </c>
       <c r="F123" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G123">
         <v>20</v>
       </c>
       <c r="H123" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -4147,7 +4154,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C124" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D124" t="s">
         <v>15</v>
@@ -4156,13 +4163,13 @@
         <v>21</v>
       </c>
       <c r="F124" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G124">
         <v>21</v>
       </c>
       <c r="H124" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -4174,7 +4181,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C125" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D125" t="s">
         <v>15</v>
@@ -4183,13 +4190,13 @@
         <v>50</v>
       </c>
       <c r="F125" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G125">
         <v>50</v>
       </c>
       <c r="H125" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -4201,7 +4208,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C126" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D126" t="s">
         <v>15</v>
@@ -4210,13 +4217,13 @@
         <v>51</v>
       </c>
       <c r="F126" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G126">
         <v>51</v>
       </c>
       <c r="H126" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -4228,7 +4235,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C127" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D127" t="s">
         <v>15</v>
@@ -4237,13 +4244,13 @@
         <v>52</v>
       </c>
       <c r="F127" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G127">
         <v>52</v>
       </c>
       <c r="H127" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -4255,7 +4262,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C128" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D128" t="s">
         <v>15</v>
@@ -4264,13 +4271,13 @@
         <v>53</v>
       </c>
       <c r="F128" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G128">
         <v>53</v>
       </c>
       <c r="H128" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -4282,7 +4289,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C129" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D129" t="s">
         <v>15</v>
@@ -4291,13 +4298,13 @@
         <v>54</v>
       </c>
       <c r="F129" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G129">
         <v>54</v>
       </c>
       <c r="H129" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -4309,7 +4316,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C130" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D130" t="s">
         <v>15</v>
@@ -4318,13 +4325,13 @@
         <v>55</v>
       </c>
       <c r="F130" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G130">
         <v>55</v>
       </c>
       <c r="H130" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -4336,7 +4343,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C131" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D131" t="s">
         <v>15</v>
@@ -4345,13 +4352,13 @@
         <v>56</v>
       </c>
       <c r="F131" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G131">
         <v>56</v>
       </c>
       <c r="H131" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -4363,7 +4370,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C132" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D132" t="s">
         <v>15</v>
@@ -4372,13 +4379,13 @@
         <v>59</v>
       </c>
       <c r="F132" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G132">
         <v>59</v>
       </c>
       <c r="H132" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -4390,7 +4397,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C133" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D133" t="s">
         <v>15</v>
@@ -4399,13 +4406,13 @@
         <v>55</v>
       </c>
       <c r="F133" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G133">
         <v>55</v>
       </c>
       <c r="H133" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
@@ -4417,7 +4424,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C134" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D134" t="s">
         <v>15</v>
@@ -4426,13 +4433,13 @@
         <v>56</v>
       </c>
       <c r="F134" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G134">
         <v>56</v>
       </c>
       <c r="H134" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
@@ -4444,7 +4451,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C135" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D135" t="s">
         <v>15</v>
@@ -4453,13 +4460,13 @@
         <v>59</v>
       </c>
       <c r="F135" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G135">
         <v>59</v>
       </c>
       <c r="H135" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -4471,7 +4478,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C136" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D136" t="s">
         <v>15</v>
@@ -4480,13 +4487,13 @@
         <v>60</v>
       </c>
       <c r="F136" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G136">
         <v>60</v>
       </c>
       <c r="H136" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -4498,7 +4505,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C137" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D137" t="s">
         <v>15</v>
@@ -4507,13 +4514,13 @@
         <v>61</v>
       </c>
       <c r="F137" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G137">
         <v>61</v>
       </c>
       <c r="H137" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
@@ -4525,7 +4532,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C138" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D138" t="s">
         <v>15</v>
@@ -4534,13 +4541,13 @@
         <v>62</v>
       </c>
       <c r="F138" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G138">
         <v>62</v>
       </c>
       <c r="H138" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
@@ -4552,7 +4559,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C139" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D139" t="s">
         <v>15</v>
@@ -4561,13 +4568,13 @@
         <v>63</v>
       </c>
       <c r="F139" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G139">
         <v>63</v>
       </c>
       <c r="H139" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
@@ -4579,7 +4586,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C140" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D140" t="s">
         <v>15</v>
@@ -4588,13 +4595,13 @@
         <v>64</v>
       </c>
       <c r="F140" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G140">
         <v>64</v>
       </c>
       <c r="H140" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
@@ -4606,7 +4613,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C141" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D141" t="s">
         <v>15</v>
@@ -4615,13 +4622,13 @@
         <v>65</v>
       </c>
       <c r="F141" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G141">
         <v>65</v>
       </c>
       <c r="H141" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
@@ -4633,7 +4640,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C142" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D142" t="s">
         <v>15</v>
@@ -4642,13 +4649,13 @@
         <v>66</v>
       </c>
       <c r="F142" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G142">
         <v>66</v>
       </c>
       <c r="H142" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
@@ -4660,7 +4667,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C143" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D143" t="s">
         <v>15</v>
@@ -4669,13 +4676,13 @@
         <v>67</v>
       </c>
       <c r="F143" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G143">
         <v>67</v>
       </c>
       <c r="H143" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
@@ -4687,7 +4694,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C144" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D144" t="s">
         <v>15</v>
@@ -4696,13 +4703,13 @@
         <v>68</v>
       </c>
       <c r="F144" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G144">
         <v>68</v>
       </c>
       <c r="H144" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
@@ -4714,7 +4721,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C145" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D145" t="s">
         <v>15</v>
@@ -4723,13 +4730,13 @@
         <v>70</v>
       </c>
       <c r="F145" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G145">
         <v>70</v>
       </c>
       <c r="H145" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
@@ -4741,7 +4748,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C146" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D146" t="s">
         <v>15</v>
@@ -4750,13 +4757,13 @@
         <v>71</v>
       </c>
       <c r="F146" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G146">
         <v>71</v>
       </c>
       <c r="H146" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
@@ -4768,7 +4775,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C147" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D147" t="s">
         <v>15</v>
@@ -4777,13 +4784,13 @@
         <v>72</v>
       </c>
       <c r="F147" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G147">
         <v>72</v>
       </c>
       <c r="H147" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
@@ -4795,7 +4802,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C148" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D148" t="s">
         <v>15</v>
@@ -4804,13 +4811,13 @@
         <v>73</v>
       </c>
       <c r="F148" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G148">
         <v>73</v>
       </c>
       <c r="H148" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
@@ -4822,7 +4829,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C149" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D149" t="s">
         <v>15</v>
@@ -4831,13 +4838,13 @@
         <v>74</v>
       </c>
       <c r="F149" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G149">
         <v>74</v>
       </c>
       <c r="H149" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -4849,7 +4856,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C150" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D150" t="s">
         <v>15</v>
@@ -4858,13 +4865,13 @@
         <v>78</v>
       </c>
       <c r="F150" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G150">
         <v>78</v>
       </c>
       <c r="H150" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
@@ -4876,7 +4883,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C151" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D151" t="s">
         <v>15</v>
@@ -4885,13 +4892,13 @@
         <v>80</v>
       </c>
       <c r="F151" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G151">
         <v>80</v>
       </c>
       <c r="H151" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
@@ -4903,7 +4910,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C152" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D152" t="s">
         <v>15</v>
@@ -4912,13 +4919,13 @@
         <v>81</v>
       </c>
       <c r="F152" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G152">
         <v>81</v>
       </c>
       <c r="H152" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
@@ -4930,7 +4937,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C153" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D153" t="s">
         <v>15</v>
@@ -4939,13 +4946,13 @@
         <v>82</v>
       </c>
       <c r="F153" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G153">
         <v>82</v>
       </c>
       <c r="H153" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
@@ -4957,7 +4964,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C154" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D154" t="s">
         <v>15</v>
@@ -4966,13 +4973,13 @@
         <v>83</v>
       </c>
       <c r="F154" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G154">
         <v>83</v>
       </c>
       <c r="H154" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
@@ -4984,7 +4991,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C155" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D155" t="s">
         <v>15</v>
@@ -4993,13 +5000,13 @@
         <v>84</v>
       </c>
       <c r="F155" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G155">
         <v>84</v>
       </c>
       <c r="H155" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
@@ -5011,7 +5018,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C156" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D156" t="s">
         <v>15</v>
@@ -5020,13 +5027,13 @@
         <v>85</v>
       </c>
       <c r="F156" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G156">
         <v>85</v>
       </c>
       <c r="H156" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
@@ -5038,7 +5045,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C157" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D157" t="s">
         <v>15</v>
@@ -5047,13 +5054,13 @@
         <v>87</v>
       </c>
       <c r="F157" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G157">
         <v>87</v>
       </c>
       <c r="H157" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
@@ -5065,7 +5072,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C158" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D158" t="s">
         <v>15</v>
@@ -5074,13 +5081,13 @@
         <v>88</v>
       </c>
       <c r="F158" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G158">
         <v>88</v>
       </c>
       <c r="H158" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
@@ -5092,7 +5099,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C159" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D159" t="s">
         <v>15</v>
@@ -5101,13 +5108,13 @@
         <v>89</v>
       </c>
       <c r="F159" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G159">
         <v>89</v>
       </c>
       <c r="H159" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
@@ -5119,7 +5126,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C160" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D160" t="s">
         <v>15</v>
@@ -5128,13 +5135,13 @@
         <v>90</v>
       </c>
       <c r="F160" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G160">
         <v>90</v>
       </c>
       <c r="H160" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
@@ -5146,7 +5153,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C161" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D161" t="s">
         <v>15</v>
@@ -5155,13 +5162,13 @@
         <v>91</v>
       </c>
       <c r="F161" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G161">
         <v>91</v>
       </c>
       <c r="H161" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
@@ -5173,7 +5180,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C162" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D162" t="s">
         <v>15</v>
@@ -5182,13 +5189,13 @@
         <v>92</v>
       </c>
       <c r="F162" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G162">
         <v>92</v>
       </c>
       <c r="H162" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
@@ -5200,7 +5207,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C163" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D163" t="s">
         <v>15</v>
@@ -5227,7 +5234,7 @@
         <v>p_crash2</v>
       </c>
       <c r="C164" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D164" t="s">
         <v>15</v>
@@ -5247,10 +5254,10 @@
         <v>6</v>
       </c>
       <c r="B165" t="s">
+        <v>217</v>
+      </c>
+      <c r="C165" t="s">
         <v>218</v>
-      </c>
-      <c r="C165" t="s">
-        <v>219</v>
       </c>
       <c r="D165" t="s">
         <v>15</v>
@@ -5259,7 +5266,7 @@
         <v>0</v>
       </c>
       <c r="F165" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G165">
         <v>0</v>
@@ -5270,10 +5277,10 @@
         <v>6</v>
       </c>
       <c r="B166" t="s">
+        <v>217</v>
+      </c>
+      <c r="C166" t="s">
         <v>218</v>
-      </c>
-      <c r="C166" t="s">
-        <v>219</v>
       </c>
       <c r="D166" t="s">
         <v>15</v>
@@ -5282,7 +5289,7 @@
         <v>1</v>
       </c>
       <c r="F166" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G166">
         <v>1</v>
@@ -5293,22 +5300,22 @@
         <v>6</v>
       </c>
       <c r="B167" t="s">
+        <v>217</v>
+      </c>
+      <c r="C167" t="s">
         <v>218</v>
       </c>
-      <c r="C167" t="s">
-        <v>219</v>
-      </c>
       <c r="D167" t="s">
         <v>15</v>
       </c>
       <c r="E167">
-        <v>2</v>
+        <v>99</v>
       </c>
       <c r="F167" t="s">
-        <v>221</v>
+        <v>47</v>
       </c>
       <c r="G167">
-        <v>9999</v>
+        <v>99</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
@@ -5316,22 +5323,22 @@
         <v>6</v>
       </c>
       <c r="B168" t="s">
+        <v>217</v>
+      </c>
+      <c r="C168" t="s">
         <v>218</v>
       </c>
-      <c r="C168" t="s">
-        <v>219</v>
-      </c>
       <c r="D168" t="s">
         <v>15</v>
       </c>
       <c r="E168">
-        <v>99</v>
+        <v>2</v>
       </c>
       <c r="F168" t="s">
-        <v>47</v>
+        <v>220</v>
       </c>
       <c r="G168">
-        <v>99</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
@@ -5339,10 +5346,10 @@
         <v>6</v>
       </c>
       <c r="B169" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C169" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D169" t="s">
         <v>15</v>
@@ -5351,7 +5358,7 @@
         <v>0</v>
       </c>
       <c r="F169" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G169">
         <v>0</v>
@@ -5362,10 +5369,10 @@
         <v>6</v>
       </c>
       <c r="B170" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C170" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D170" t="s">
         <v>15</v>
@@ -5374,7 +5381,7 @@
         <v>1</v>
       </c>
       <c r="F170" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G170">
         <v>1</v>
@@ -5385,10 +5392,10 @@
         <v>6</v>
       </c>
       <c r="B171" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C171" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D171" t="s">
         <v>15</v>
@@ -5397,7 +5404,7 @@
         <v>2</v>
       </c>
       <c r="F171" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G171">
         <v>2</v>
@@ -5408,10 +5415,10 @@
         <v>6</v>
       </c>
       <c r="B172" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C172" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D172" t="s">
         <v>15</v>
@@ -5420,7 +5427,7 @@
         <v>3</v>
       </c>
       <c r="F172" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G172">
         <v>3</v>
@@ -5431,10 +5438,10 @@
         <v>6</v>
       </c>
       <c r="B173" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C173" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D173" t="s">
         <v>15</v>
@@ -5443,7 +5450,7 @@
         <v>4</v>
       </c>
       <c r="F173" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G173">
         <v>4</v>
@@ -5454,10 +5461,10 @@
         <v>6</v>
       </c>
       <c r="B174" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C174" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D174" t="s">
         <v>15</v>
@@ -5466,7 +5473,7 @@
         <v>5</v>
       </c>
       <c r="F174" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G174">
         <v>5</v>
@@ -5477,10 +5484,10 @@
         <v>6</v>
       </c>
       <c r="B175" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C175" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D175" t="s">
         <v>15</v>
@@ -5489,7 +5496,7 @@
         <v>6</v>
       </c>
       <c r="F175" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G175">
         <v>6</v>
@@ -5500,10 +5507,10 @@
         <v>6</v>
       </c>
       <c r="B176" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C176" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D176" t="s">
         <v>15</v>
@@ -5512,7 +5519,7 @@
         <v>7</v>
       </c>
       <c r="F176" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G176">
         <v>7</v>
@@ -5523,10 +5530,10 @@
         <v>6</v>
       </c>
       <c r="B177" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C177" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D177" t="s">
         <v>15</v>
@@ -5546,10 +5553,10 @@
         <v>6</v>
       </c>
       <c r="B178" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C178" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D178" t="s">
         <v>15</v>
@@ -5558,13 +5565,13 @@
         <v>13</v>
       </c>
       <c r="F178" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G178">
         <v>13</v>
       </c>
       <c r="H178" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
@@ -5572,10 +5579,10 @@
         <v>6</v>
       </c>
       <c r="B179" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C179" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D179" t="s">
         <v>15</v>
@@ -5584,13 +5591,13 @@
         <v>1</v>
       </c>
       <c r="F179" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G179">
         <v>1</v>
       </c>
       <c r="H179" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.25">
@@ -5598,25 +5605,25 @@
         <v>6</v>
       </c>
       <c r="B180" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C180" t="s">
+        <v>230</v>
+      </c>
+      <c r="D180" t="s">
+        <v>15</v>
+      </c>
+      <c r="E180">
+        <v>6</v>
+      </c>
+      <c r="F180" t="s">
         <v>231</v>
       </c>
-      <c r="D180" t="s">
-        <v>15</v>
-      </c>
-      <c r="E180">
-        <v>6</v>
-      </c>
-      <c r="F180" t="s">
+      <c r="G180">
+        <v>6</v>
+      </c>
+      <c r="H180" t="s">
         <v>232</v>
-      </c>
-      <c r="G180">
-        <v>6</v>
-      </c>
-      <c r="H180" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
@@ -5624,10 +5631,10 @@
         <v>6</v>
       </c>
       <c r="B181" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C181" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D181" t="s">
         <v>15</v>
@@ -5636,13 +5643,13 @@
         <v>50</v>
       </c>
       <c r="F181" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G181">
         <v>50</v>
       </c>
       <c r="H181" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
@@ -5650,10 +5657,10 @@
         <v>6</v>
       </c>
       <c r="B182" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C182" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D182" t="s">
         <v>15</v>
@@ -5662,13 +5669,13 @@
         <v>51</v>
       </c>
       <c r="F182" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G182">
         <v>51</v>
       </c>
       <c r="H182" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.25">
@@ -5676,25 +5683,25 @@
         <v>6</v>
       </c>
       <c r="B183" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C183" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D183" t="s">
         <v>15</v>
       </c>
       <c r="E183">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F183" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="G183">
-        <v>9999</v>
+        <v>99</v>
       </c>
       <c r="H183" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
@@ -5702,36 +5709,36 @@
         <v>6</v>
       </c>
       <c r="B184" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C184" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D184" t="s">
         <v>15</v>
       </c>
       <c r="E184">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F184" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="G184">
-        <v>99</v>
+        <v>9999</v>
       </c>
       <c r="H184" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
+        <v>237</v>
+      </c>
+      <c r="B185" t="s">
         <v>238</v>
       </c>
-      <c r="B185" t="s">
+      <c r="C185" t="s">
         <v>239</v>
-      </c>
-      <c r="C185" t="s">
-        <v>240</v>
       </c>
       <c r="D185" t="s">
         <v>15</v>
@@ -5740,7 +5747,7 @@
         <v>1</v>
       </c>
       <c r="F185" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G185">
         <v>1</v>
@@ -5748,13 +5755,13 @@
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
+        <v>237</v>
+      </c>
+      <c r="B186" t="s">
         <v>238</v>
       </c>
-      <c r="B186" t="s">
+      <c r="C186" t="s">
         <v>239</v>
-      </c>
-      <c r="C186" t="s">
-        <v>240</v>
       </c>
       <c r="D186" t="s">
         <v>15</v>
@@ -5771,13 +5778,13 @@
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B187" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C187" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D187" t="s">
         <v>15</v>
@@ -5786,7 +5793,7 @@
         <v>99</v>
       </c>
       <c r="F187" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G187">
         <v>99</v>
@@ -5794,13 +5801,13 @@
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B188" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C188" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D188" t="s">
         <v>15</v>
@@ -5809,7 +5816,7 @@
         <v>1</v>
       </c>
       <c r="F188" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G188">
         <v>1</v>
@@ -5817,13 +5824,13 @@
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B189" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C189" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D189" t="s">
         <v>15</v>
@@ -5832,7 +5839,7 @@
         <v>2</v>
       </c>
       <c r="F189" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G189">
         <v>2</v>
@@ -5840,13 +5847,13 @@
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B190" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C190" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D190" t="s">
         <v>15</v>
@@ -5855,7 +5862,7 @@
         <v>3</v>
       </c>
       <c r="F190" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G190">
         <v>3</v>
@@ -5863,13 +5870,13 @@
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B191" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C191" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D191" t="s">
         <v>15</v>
@@ -5878,7 +5885,7 @@
         <v>4</v>
       </c>
       <c r="F191" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G191">
         <v>4</v>
@@ -5886,13 +5893,13 @@
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B192" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C192" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D192" t="s">
         <v>15</v>
@@ -5901,7 +5908,7 @@
         <v>5</v>
       </c>
       <c r="F192" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G192">
         <v>5</v>
@@ -5909,13 +5916,13 @@
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B193" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C193" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D193" t="s">
         <v>15</v>
@@ -5924,7 +5931,7 @@
         <v>6</v>
       </c>
       <c r="F193" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G193">
         <v>6</v>
@@ -5932,13 +5939,13 @@
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B194" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C194" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D194" t="s">
         <v>15</v>
@@ -5955,13 +5962,13 @@
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B195" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C195" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D195" t="s">
         <v>15</v>
@@ -5970,7 +5977,7 @@
         <v>1</v>
       </c>
       <c r="F195" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G195">
         <v>1</v>
@@ -5978,13 +5985,13 @@
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B196" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C196" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D196" t="s">
         <v>15</v>
@@ -5993,7 +6000,7 @@
         <v>2</v>
       </c>
       <c r="F196" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G196">
         <v>2</v>
@@ -6001,13 +6008,13 @@
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B197" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C197" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D197" t="s">
         <v>15</v>
@@ -6016,7 +6023,7 @@
         <v>3</v>
       </c>
       <c r="F197" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G197">
         <v>3</v>
@@ -6024,13 +6031,13 @@
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B198" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C198" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D198" t="s">
         <v>15</v>
@@ -6039,7 +6046,7 @@
         <v>4</v>
       </c>
       <c r="F198" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G198">
         <v>4</v>
@@ -6047,13 +6054,13 @@
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B199" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C199" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D199" t="s">
         <v>15</v>
@@ -6062,7 +6069,7 @@
         <v>5</v>
       </c>
       <c r="F199" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G199">
         <v>5</v>
@@ -6070,13 +6077,13 @@
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B200" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C200" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D200" t="s">
         <v>15</v>
@@ -6085,7 +6092,7 @@
         <v>6</v>
       </c>
       <c r="F200" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G200">
         <v>6</v>
@@ -6093,13 +6100,13 @@
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B201" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C201" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D201" t="s">
         <v>15</v>
@@ -6116,13 +6123,13 @@
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B202" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C202" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D202" t="s">
         <v>15</v>
@@ -6131,7 +6138,7 @@
         <v>99</v>
       </c>
       <c r="F202" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G202">
         <v>99</v>
@@ -6139,13 +6146,13 @@
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B203" t="s">
+        <v>250</v>
+      </c>
+      <c r="C203" t="s">
         <v>251</v>
-      </c>
-      <c r="C203" t="s">
-        <v>252</v>
       </c>
       <c r="D203" t="s">
         <v>15</v>
@@ -6154,7 +6161,7 @@
         <v>1</v>
       </c>
       <c r="F203" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G203">
         <v>1</v>
@@ -6162,13 +6169,13 @@
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B204" t="s">
+        <v>250</v>
+      </c>
+      <c r="C204" t="s">
         <v>251</v>
-      </c>
-      <c r="C204" t="s">
-        <v>252</v>
       </c>
       <c r="D204" t="s">
         <v>15</v>
@@ -6177,7 +6184,7 @@
         <v>2</v>
       </c>
       <c r="F204" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G204">
         <v>2</v>
@@ -6185,13 +6192,13 @@
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B205" t="s">
+        <v>250</v>
+      </c>
+      <c r="C205" t="s">
         <v>251</v>
-      </c>
-      <c r="C205" t="s">
-        <v>252</v>
       </c>
       <c r="D205" t="s">
         <v>15</v>
@@ -6208,13 +6215,13 @@
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B206" t="s">
+        <v>250</v>
+      </c>
+      <c r="C206" t="s">
         <v>251</v>
-      </c>
-      <c r="C206" t="s">
-        <v>252</v>
       </c>
       <c r="D206" t="s">
         <v>15</v>
@@ -6234,10 +6241,10 @@
         <v>6</v>
       </c>
       <c r="B207" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C207" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D207" t="s">
         <v>15</v>
@@ -6246,10 +6253,10 @@
         <v>1</v>
       </c>
       <c r="F207" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G207" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.25">
@@ -6257,10 +6264,10 @@
         <v>6</v>
       </c>
       <c r="B208" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C208" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D208" t="s">
         <v>15</v>
@@ -6269,10 +6276,10 @@
         <v>2</v>
       </c>
       <c r="F208" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G208" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
@@ -6280,10 +6287,10 @@
         <v>6</v>
       </c>
       <c r="B209" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C209" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D209" t="s">
         <v>15</v>
@@ -6292,10 +6299,10 @@
         <v>3</v>
       </c>
       <c r="F209" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G209" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
@@ -6303,10 +6310,10 @@
         <v>6</v>
       </c>
       <c r="B210" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C210" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D210" t="s">
         <v>15</v>
@@ -6315,10 +6322,10 @@
         <v>4</v>
       </c>
       <c r="F210" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G210" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
@@ -6326,10 +6333,10 @@
         <v>6</v>
       </c>
       <c r="B211" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C211" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D211" t="s">
         <v>15</v>
@@ -6338,10 +6345,10 @@
         <v>5</v>
       </c>
       <c r="F211" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G211" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
@@ -6349,10 +6356,10 @@
         <v>6</v>
       </c>
       <c r="B212" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C212" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D212" t="s">
         <v>15</v>
@@ -6361,10 +6368,10 @@
         <v>6</v>
       </c>
       <c r="F212" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G212" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
@@ -6372,10 +6379,10 @@
         <v>6</v>
       </c>
       <c r="B213" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C213" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D213" t="s">
         <v>15</v>
@@ -6384,7 +6391,7 @@
         <v>7</v>
       </c>
       <c r="F213" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G213">
         <v>850</v>
@@ -6395,10 +6402,10 @@
         <v>6</v>
       </c>
       <c r="B214" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C214" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D214" t="s">
         <v>15</v>
@@ -6407,10 +6414,10 @@
         <v>8</v>
       </c>
       <c r="F214" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G214" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
@@ -6418,10 +6425,10 @@
         <v>6</v>
       </c>
       <c r="B215" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C215" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D215" t="s">
         <v>15</v>
@@ -6433,7 +6440,7 @@
         <v>40</v>
       </c>
       <c r="G215" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
@@ -6441,10 +6448,10 @@
         <v>6</v>
       </c>
       <c r="B216" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C216" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D216" t="s">
         <v>15</v>
@@ -6453,7 +6460,7 @@
         <v>998</v>
       </c>
       <c r="F216" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G216">
         <v>998</v>
@@ -6464,10 +6471,10 @@
         <v>6</v>
       </c>
       <c r="B217" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C217" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D217" t="s">
         <v>15</v>
@@ -6476,7 +6483,7 @@
         <v>999</v>
       </c>
       <c r="F217" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G217" s="2">
         <v>997998</v>
@@ -6493,7 +6500,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6544,10 +6551,10 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="s">
         <v>61</v>
-      </c>
-      <c r="D4" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -6555,10 +6562,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" t="s">
         <v>111</v>
-      </c>
-      <c r="D5" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>